<commit_message>
Auto-save via app Streamlit
</commit_message>
<xml_diff>
--- a/reservations.xlsx
+++ b/reservations.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2893,33 +2893,80 @@
       <c r="O50" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr"/>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Claudine Fleury</t>
+        </is>
+      </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr"/>
-      <c r="F51" t="inlineStr"/>
+          <t>Booking</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>+33334691787</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>46200</v>
+      </c>
+      <c r="E51" s="2" t="n">
+        <v>46203</v>
+      </c>
+      <c r="F51" t="n">
+        <v>3</v>
+      </c>
       <c r="G51" t="n">
-        <v>16753.96</v>
+        <v>468.68</v>
       </c>
       <c r="H51" t="n">
-        <v>13833.27</v>
+        <v>374.77</v>
       </c>
       <c r="I51" t="n">
-        <v>2920.69</v>
+        <v>93.91</v>
       </c>
       <c r="J51" t="n">
-        <v>17.43</v>
-      </c>
-      <c r="K51" t="inlineStr"/>
-      <c r="L51" t="inlineStr"/>
+        <v>20.04</v>
+      </c>
+      <c r="K51" t="n">
+        <v>2026</v>
+      </c>
+      <c r="L51" t="n">
+        <v>6</v>
+      </c>
       <c r="M51" t="inlineStr"/>
       <c r="N51" t="inlineStr"/>
       <c r="O51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="n">
+        <v>16753.96</v>
+      </c>
+      <c r="H52" t="n">
+        <v>13833.27</v>
+      </c>
+      <c r="I52" t="n">
+        <v>2920.69</v>
+      </c>
+      <c r="J52" t="n">
+        <v>17.43</v>
+      </c>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Test push manuel depuis l'app
</commit_message>
<xml_diff>
--- a/reservations.xlsx
+++ b/reservations.xlsx
@@ -2903,10 +2903,8 @@
           <t>Booking</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>+33334691787</t>
-        </is>
+      <c r="C51" t="n">
+        <v>33334691787</v>
       </c>
       <c r="D51" s="2" t="n">
         <v>46200</v>

</xml_diff>